<commit_message>
vaccination added to the Simulation
</commit_message>
<xml_diff>
--- a/WIP/Adding_vaccination/output.xlsx
+++ b/WIP/Adding_vaccination/output.xlsx
@@ -423,25 +423,25 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>32</v>
+        <v>61.5</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -450,19 +450,19 @@
         <v>0.1</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>61.5</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -471,19 +471,19 @@
         <v>0.2</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -492,19 +492,19 @@
         <v>0.3</v>
       </c>
       <c r="C5">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -513,19 +513,19 @@
         <v>0.4</v>
       </c>
       <c r="C6">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -534,19 +534,19 @@
         <v>0.5</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -555,19 +555,19 @@
         <v>0.6</v>
       </c>
       <c r="C8">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D8">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -576,19 +576,19 @@
         <v>0.7</v>
       </c>
       <c r="C9">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="D9">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -597,19 +597,19 @@
         <v>0.7999999999999999</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="D10">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -618,19 +618,19 @@
         <v>0.8999999999999999</v>
       </c>
       <c r="C11">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E11">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -639,42 +639,42 @@
         <v>0.9999999999999999</v>
       </c>
       <c r="C12">
+        <v>33</v>
+      </c>
+      <c r="D12">
         <v>8</v>
       </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
       <c r="E12">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
-        <v>0.3</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -683,19 +683,19 @@
         <v>0.1</v>
       </c>
       <c r="C14">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -704,19 +704,19 @@
         <v>0.2</v>
       </c>
       <c r="C15">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -725,19 +725,19 @@
         <v>0.3</v>
       </c>
       <c r="C16">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -746,19 +746,19 @@
         <v>0.4</v>
       </c>
       <c r="C17">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -767,19 +767,19 @@
         <v>0.5</v>
       </c>
       <c r="C18">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D18">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -788,19 +788,19 @@
         <v>0.6</v>
       </c>
       <c r="C19">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -812,16 +812,16 @@
         <v>51</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -830,19 +830,19 @@
         <v>0.7999999999999999</v>
       </c>
       <c r="C21">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F21">
         <v>3</v>
       </c>
       <c r="G21">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -851,10 +851,10 @@
         <v>0.8999999999999999</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <v>6</v>
@@ -863,7 +863,7 @@
         <v>3</v>
       </c>
       <c r="G22">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -875,16 +875,16 @@
         <v>40</v>
       </c>
       <c r="D23">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E23">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F23">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G23">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>